<commit_message>
added some parametric models
</commit_message>
<xml_diff>
--- a/models/dft/dcas/parameters.xlsx
+++ b/models/dft/dcas/parameters.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
-    <sheet name="Properties" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -38,9 +37,6 @@
   </si>
   <si>
     <t>inverse</t>
-  </si>
-  <si>
-    <t>failed</t>
   </si>
   <si>
     <t>P</t>
@@ -391,7 +387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -416,7 +412,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -434,7 +430,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -452,7 +448,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -470,7 +466,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -488,7 +484,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -506,7 +502,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -524,7 +520,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -542,7 +538,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -560,7 +556,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -578,7 +574,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -641,176 +637,6 @@
     <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>26000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>28000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>29000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>30000</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
few changes in scenario LP
</commit_message>
<xml_diff>
--- a/models/dft/dcas/parameters.xlsx
+++ b/models/dft/dcas/parameters.xlsx
@@ -388,7 +388,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,8 +421,8 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="D2" s="1">
-        <f>C2/3</f>
-        <v>1.6666666666666667E-5</v>
+        <f>C2/2</f>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -439,8 +439,8 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D11" si="0">C3/3</f>
-        <v>1.6666666666666667E-5</v>
+        <f t="shared" ref="D3:D11" si="0">C3/2</f>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -458,7 +458,7 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>6.6666666666666675E-6</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -476,7 +476,7 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>6.6666666666666675E-6</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -494,7 +494,7 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>3.333333333333333E-7</v>
+        <v>4.9999999999999998E-7</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -512,7 +512,7 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -530,7 +530,7 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -566,7 +566,7 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -584,7 +584,7 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>

</xml_diff>